<commit_message>
Finished black box testing
</commit_message>
<xml_diff>
--- a/TruckDelivery/Documents/Testing/Black Box Test.xlsx
+++ b/TruckDelivery/Documents/Testing/Black Box Test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7db8d14ad41d10d3/CPA/S2/SFT221/Project/TruckDelivery/Documents/Testing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9419027ddbc790ca/Desktop/SFT221/Project/Win23-SFT221-NDD-1-main/Win23-SFT221-NDD-1/TruckDelivery/Documents/Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="548" documentId="8_{2B0D13F8-605D-4477-A3F3-78053347296E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96EAEEBB-D9AA-42C7-8291-71C0F088709B}"/>
+  <xr:revisionPtr revIDLastSave="570" documentId="8_{2B0D13F8-605D-4477-A3F3-78053347296E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{642E96F0-46A4-4B38-902E-ED84E1DCA377}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="4410" windowWidth="20640" windowHeight="11040" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Declaration" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="39">
   <si>
     <t>SFT 221</t>
   </si>
@@ -159,6 +159,46 @@
   </si>
   <si>
     <t>Testing the exit input.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">		do {
+			printf("Enter shipment weight, box size and destination (0 0 x to stop): ");
+			scanf("%d %2.1f %3[^\n]", &amp;shipment-&gt;m_weight, &amp;shipment-&gt;m_size, shipment-&gt;m_destination);
+			if (!shipment-&gt;m_weight &amp;&amp; !shipment-&gt;m_size &amp;&amp; shipment-&gt;m_destination[0] == 'x') {//exit condit
+				flag = 1;
+				break;
+			} 
+			scanf(shipment-&gt;m_destination, "%d%c", &amp;yAxis, &amp;xAxis);//parse string
+			if (shipment-&gt;m_weight &lt; MIN_WEIGHT || shipment-&gt;m_weight &gt; MAX_WEIGHT) {
+				printf("Invalid weight (must be 1-1000 Kg.)\n");
+			}
+			if (shipment-&gt;m_size &lt; MIN_SIZE || shipment-&gt;m_size &gt; MAX_SIZE) {
+				printf("Invalid size\n");
+			}
+			if (yAxis &lt; MIN_YAXIS || yAxis &gt; MAX_YAXIS || xAxis &lt; 'a' || xAxis &gt; 'y') {
+				printf("Invalid destination\n");
+			}
+		} while (shipment-&gt;m_weight &lt; MIN_WEIGHT || shipment-&gt;m_weight &gt; MAX_WEIGHT ||
+			shipment-&gt;m_size &lt; MIN_SIZE || shipment-&gt;m_size &gt; MAX_SIZE ||
+			yAxis &lt; MIN_YAXIS || yAxis &gt; MAX_YAXIS || xAxis &lt; 'a' || xAxis &gt; 'y');</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Code exited properly</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> When inputing value over the range for kg, size and destination, error message shows properly</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Will not accept whitespace characters as inputs and will only accept 3 values as inputs</t>
   </si>
 </sst>
 </file>
@@ -381,10 +421,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -744,6 +780,316 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61924722-0D75-4F1E-8D57-22B9AFF38D7F}">
   <dimension ref="A2:C14"/>
   <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" customWidth="1"/>
+    <col min="3" max="3" width="73" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="390" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F91D8E0-EF0F-4156-A77F-40F43871CAA6}">
+  <dimension ref="A2:C14"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" customWidth="1"/>
+    <col min="3" max="3" width="73" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="390" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41BA5EDD-46C3-42C0-98A8-FAEFD0B55497}">
+  <dimension ref="A2:C14"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" customWidth="1"/>
+    <col min="3" max="3" width="73" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="390" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7569972F-F81D-4231-8C70-489229E9D248}">
+  <dimension ref="A2:C14"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" customWidth="1"/>
+    <col min="3" max="3" width="73" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="390" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249C1705-E2BE-4F34-9A6A-AC67B43C9589}">
+  <dimension ref="A2:C14"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
@@ -760,7 +1106,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -768,7 +1114,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -791,7 +1137,9 @@
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -813,12 +1161,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F91D8E0-EF0F-4156-A77F-40F43871CAA6}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E656B9-DA9B-4F4A-B0FF-2C5AA8A7857B}">
   <dimension ref="A2:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,15 +1181,15 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -864,305 +1212,17 @@
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41BA5EDD-46C3-42C0-98A8-FAEFD0B55497}">
-  <dimension ref="A2:C14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.85546875" customWidth="1"/>
-    <col min="3" max="3" width="73" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="390" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7569972F-F81D-4231-8C70-489229E9D248}">
-  <dimension ref="A2:C14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.85546875" customWidth="1"/>
-    <col min="3" max="3" width="73" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="390" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249C1705-E2BE-4F34-9A6A-AC67B43C9589}">
-  <dimension ref="A2:C14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.85546875" customWidth="1"/>
-    <col min="3" max="3" width="73" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="390" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E656B9-DA9B-4F4A-B0FF-2C5AA8A7857B}">
-  <dimension ref="A2:C14"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.85546875" customWidth="1"/>
-    <col min="3" max="3" width="73" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="390" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
@@ -1234,26 +1294,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="7db3b190-d1cf-4882-bee6-3064ce691739" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100068B9DB3898E1840A1985BE38A336A09" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6986600eeaa410782a35a751b922af63">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b" xmlns:ns3="7db3b190-d1cf-4882-bee6-3064ce691739" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bcc5f470bd5cdaad943a5d943b97cad8" ns2:_="" ns3:_="">
     <xsd:import namespace="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b"/>
@@ -1436,26 +1476,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="7db3b190-d1cf-4882-bee6-3064ce691739" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D20CED7A-A184-4DAD-98D0-D68B5D737C5B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7db3b190-d1cf-4882-bee6-3064ce691739"/>
-    <ds:schemaRef ds:uri="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A445DA8-61DA-4B15-A75B-C715E0A15404}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{474F1F35-2E98-4F8D-A6FA-19110723F686}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1472,4 +1513,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A445DA8-61DA-4B15-A75B-C715E0A15404}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D20CED7A-A184-4DAD-98D0-D68B5D737C5B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7db3b190-d1cf-4882-bee6-3064ce691739"/>
+    <ds:schemaRef ds:uri="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>